<commit_message>
fix debug issues, fix excel file path
</commit_message>
<xml_diff>
--- a/TestPractice/Data/Login.xlsx
+++ b/TestPractice/Data/Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tolo\source\repos\FrameworkBase\TestPractice\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E2248E-1EB3-4850-98D7-5FC98B63D832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52E3896-6956-4F54-848B-00F35BB34A22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,23 +27,23 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>userName</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
     <t>lolo_tol_10@hotmail.com</t>
   </si>
   <si>
-    <t>TestPass123</t>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>TestingPass123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +55,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,9 +89,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -377,16 +386,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -397,5 +406,6 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{4B86D975-7B5E-4953-B709-8A4EB395147C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>